<commit_message>
added sound and recogResp times
</commit_message>
<xml_diff>
--- a/syncTemplate.xlsx
+++ b/syncTemplate.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="689">
   <si>
     <t>label</t>
   </si>
@@ -1877,6 +1877,222 @@
   </si>
   <si>
     <t>fin</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_2</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_3</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_4</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_5</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_6</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_7</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_8</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_9</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_10</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_11</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_12</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_13</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_14</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_15</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_16</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_17</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_18</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_19</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_20</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_21</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_22</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_23</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_24</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_25</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_26</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_27</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_28</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_29</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_30</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_31</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_32</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_33</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_34</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_35</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_36</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_37</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_38</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_39</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_40</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_41</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_42</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_43</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_44</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_45</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_46</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_47</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_48</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_49</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_50</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_51</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_52</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_53</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_54</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_55</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_56</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_57</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_58</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_59</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_60</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_61</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_62</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_63</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_64</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_65</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_66</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_67</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_68</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_69</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_70</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_71</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_72</t>
+  </si>
+  <si>
+    <t>emotionMem_recogDispTime_1</t>
   </si>
 </sst>
 </file>
@@ -2229,10 +2445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D701"/>
+  <dimension ref="A1:D845"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="A535" sqref="A535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -7875,6 +8091,1158 @@
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A701" t="s">
+        <v>688</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A702" t="s">
+        <v>7</v>
+      </c>
+      <c r="B702" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="703" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A703" t="s">
+        <v>617</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A704" t="s">
+        <v>7</v>
+      </c>
+      <c r="B704" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A705" t="s">
+        <v>618</v>
+      </c>
+      <c r="B705" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A706" t="s">
+        <v>7</v>
+      </c>
+      <c r="B706" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A707" t="s">
+        <v>619</v>
+      </c>
+      <c r="B707" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A708" t="s">
+        <v>7</v>
+      </c>
+      <c r="B708" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A709" t="s">
+        <v>620</v>
+      </c>
+      <c r="B709" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A710" t="s">
+        <v>7</v>
+      </c>
+      <c r="B710" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A711" t="s">
+        <v>621</v>
+      </c>
+      <c r="B711" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A712" t="s">
+        <v>7</v>
+      </c>
+      <c r="B712" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A713" t="s">
+        <v>622</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A714" t="s">
+        <v>7</v>
+      </c>
+      <c r="B714" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A715" t="s">
+        <v>623</v>
+      </c>
+      <c r="B715" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A716" t="s">
+        <v>7</v>
+      </c>
+      <c r="B716" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A717" t="s">
+        <v>624</v>
+      </c>
+      <c r="B717" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A718" t="s">
+        <v>7</v>
+      </c>
+      <c r="B718" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A719" t="s">
+        <v>625</v>
+      </c>
+      <c r="B719" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A720" t="s">
+        <v>7</v>
+      </c>
+      <c r="B720" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A721" t="s">
+        <v>626</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A722" t="s">
+        <v>7</v>
+      </c>
+      <c r="B722" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A723" t="s">
+        <v>627</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A724" t="s">
+        <v>7</v>
+      </c>
+      <c r="B724" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A725" t="s">
+        <v>628</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A726" t="s">
+        <v>7</v>
+      </c>
+      <c r="B726" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A727" t="s">
+        <v>629</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A728" t="s">
+        <v>7</v>
+      </c>
+      <c r="B728" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A729" t="s">
+        <v>630</v>
+      </c>
+      <c r="B729" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A730" t="s">
+        <v>7</v>
+      </c>
+      <c r="B730" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A731" t="s">
+        <v>631</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A732" t="s">
+        <v>7</v>
+      </c>
+      <c r="B732" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A733" t="s">
+        <v>632</v>
+      </c>
+      <c r="B733" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A734" t="s">
+        <v>7</v>
+      </c>
+      <c r="B734" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A735" t="s">
+        <v>633</v>
+      </c>
+      <c r="B735" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A736" t="s">
+        <v>7</v>
+      </c>
+      <c r="B736" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A737" t="s">
+        <v>634</v>
+      </c>
+      <c r="B737" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A738" t="s">
+        <v>7</v>
+      </c>
+      <c r="B738" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A739" t="s">
+        <v>635</v>
+      </c>
+      <c r="B739" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A740" t="s">
+        <v>7</v>
+      </c>
+      <c r="B740" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A741" t="s">
+        <v>636</v>
+      </c>
+      <c r="B741" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A742" t="s">
+        <v>7</v>
+      </c>
+      <c r="B742" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A743" t="s">
+        <v>637</v>
+      </c>
+      <c r="B743" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A744" t="s">
+        <v>7</v>
+      </c>
+      <c r="B744" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A745" t="s">
+        <v>638</v>
+      </c>
+      <c r="B745" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A746" t="s">
+        <v>7</v>
+      </c>
+      <c r="B746" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A747" t="s">
+        <v>639</v>
+      </c>
+      <c r="B747" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A748" t="s">
+        <v>7</v>
+      </c>
+      <c r="B748" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A749" t="s">
+        <v>640</v>
+      </c>
+      <c r="B749" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A750" t="s">
+        <v>7</v>
+      </c>
+      <c r="B750" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A751" t="s">
+        <v>641</v>
+      </c>
+      <c r="B751" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A752" t="s">
+        <v>7</v>
+      </c>
+      <c r="B752" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A753" t="s">
+        <v>642</v>
+      </c>
+      <c r="B753" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A754" t="s">
+        <v>7</v>
+      </c>
+      <c r="B754" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A755" t="s">
+        <v>643</v>
+      </c>
+      <c r="B755" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A756" t="s">
+        <v>7</v>
+      </c>
+      <c r="B756" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A757" t="s">
+        <v>644</v>
+      </c>
+      <c r="B757" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A758" t="s">
+        <v>7</v>
+      </c>
+      <c r="B758" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A759" t="s">
+        <v>645</v>
+      </c>
+      <c r="B759" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A760" t="s">
+        <v>7</v>
+      </c>
+      <c r="B760" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A761" t="s">
+        <v>646</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A762" t="s">
+        <v>7</v>
+      </c>
+      <c r="B762" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A763" t="s">
+        <v>647</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A764" t="s">
+        <v>7</v>
+      </c>
+      <c r="B764" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A765" t="s">
+        <v>648</v>
+      </c>
+      <c r="B765" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A766" t="s">
+        <v>7</v>
+      </c>
+      <c r="B766" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A767" t="s">
+        <v>649</v>
+      </c>
+      <c r="B767" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A768" t="s">
+        <v>7</v>
+      </c>
+      <c r="B768" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A769" t="s">
+        <v>650</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A770" t="s">
+        <v>7</v>
+      </c>
+      <c r="B770" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A771" t="s">
+        <v>651</v>
+      </c>
+      <c r="B771" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A772" t="s">
+        <v>7</v>
+      </c>
+      <c r="B772" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A773" t="s">
+        <v>652</v>
+      </c>
+      <c r="B773" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A774" t="s">
+        <v>7</v>
+      </c>
+      <c r="B774" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A775" t="s">
+        <v>653</v>
+      </c>
+      <c r="B775" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A776" t="s">
+        <v>7</v>
+      </c>
+      <c r="B776" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A777" t="s">
+        <v>654</v>
+      </c>
+      <c r="B777" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A778" t="s">
+        <v>7</v>
+      </c>
+      <c r="B778" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A779" t="s">
+        <v>655</v>
+      </c>
+      <c r="B779" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A780" t="s">
+        <v>7</v>
+      </c>
+      <c r="B780" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A781" t="s">
+        <v>656</v>
+      </c>
+      <c r="B781" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A782" t="s">
+        <v>7</v>
+      </c>
+      <c r="B782" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A783" t="s">
+        <v>657</v>
+      </c>
+      <c r="B783" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A784" t="s">
+        <v>7</v>
+      </c>
+      <c r="B784" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A785" t="s">
+        <v>658</v>
+      </c>
+      <c r="B785" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A786" t="s">
+        <v>7</v>
+      </c>
+      <c r="B786" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A787" t="s">
+        <v>659</v>
+      </c>
+      <c r="B787" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A788" t="s">
+        <v>7</v>
+      </c>
+      <c r="B788" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A789" t="s">
+        <v>660</v>
+      </c>
+      <c r="B789" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A790" t="s">
+        <v>7</v>
+      </c>
+      <c r="B790" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A791" t="s">
+        <v>661</v>
+      </c>
+      <c r="B791" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A792" t="s">
+        <v>7</v>
+      </c>
+      <c r="B792" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A793" t="s">
+        <v>662</v>
+      </c>
+      <c r="B793" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A794" t="s">
+        <v>7</v>
+      </c>
+      <c r="B794" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A795" t="s">
+        <v>663</v>
+      </c>
+      <c r="B795" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A796" t="s">
+        <v>7</v>
+      </c>
+      <c r="B796" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A797" t="s">
+        <v>664</v>
+      </c>
+      <c r="B797" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A798" t="s">
+        <v>7</v>
+      </c>
+      <c r="B798" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A799" t="s">
+        <v>665</v>
+      </c>
+      <c r="B799" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A800" t="s">
+        <v>7</v>
+      </c>
+      <c r="B800" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="801" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A801" t="s">
+        <v>666</v>
+      </c>
+      <c r="B801" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A802" t="s">
+        <v>7</v>
+      </c>
+      <c r="B802" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A803" t="s">
+        <v>667</v>
+      </c>
+      <c r="B803" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A804" t="s">
+        <v>7</v>
+      </c>
+      <c r="B804" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A805" t="s">
+        <v>668</v>
+      </c>
+      <c r="B805" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A806" t="s">
+        <v>7</v>
+      </c>
+      <c r="B806" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A807" t="s">
+        <v>669</v>
+      </c>
+      <c r="B807" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A808" t="s">
+        <v>7</v>
+      </c>
+      <c r="B808" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A809" t="s">
+        <v>670</v>
+      </c>
+      <c r="B809" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A810" t="s">
+        <v>7</v>
+      </c>
+      <c r="B810" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A811" t="s">
+        <v>671</v>
+      </c>
+      <c r="B811" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A812" t="s">
+        <v>7</v>
+      </c>
+      <c r="B812" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A813" t="s">
+        <v>672</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A814" t="s">
+        <v>7</v>
+      </c>
+      <c r="B814" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A815" t="s">
+        <v>673</v>
+      </c>
+      <c r="B815" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A816" t="s">
+        <v>7</v>
+      </c>
+      <c r="B816" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A817" t="s">
+        <v>674</v>
+      </c>
+      <c r="B817" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A818" t="s">
+        <v>7</v>
+      </c>
+      <c r="B818" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A819" t="s">
+        <v>675</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A820" t="s">
+        <v>7</v>
+      </c>
+      <c r="B820" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A821" t="s">
+        <v>676</v>
+      </c>
+      <c r="B821" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A822" t="s">
+        <v>7</v>
+      </c>
+      <c r="B822" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A823" t="s">
+        <v>677</v>
+      </c>
+      <c r="B823" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A824" t="s">
+        <v>7</v>
+      </c>
+      <c r="B824" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A825" t="s">
+        <v>678</v>
+      </c>
+      <c r="B825" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A826" t="s">
+        <v>7</v>
+      </c>
+      <c r="B826" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A827" t="s">
+        <v>679</v>
+      </c>
+      <c r="B827" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A828" t="s">
+        <v>7</v>
+      </c>
+      <c r="B828" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A829" t="s">
+        <v>680</v>
+      </c>
+      <c r="B829" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A830" t="s">
+        <v>7</v>
+      </c>
+      <c r="B830" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A831" t="s">
+        <v>681</v>
+      </c>
+      <c r="B831" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A832" t="s">
+        <v>7</v>
+      </c>
+      <c r="B832" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A833" t="s">
+        <v>682</v>
+      </c>
+      <c r="B833" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A834" t="s">
+        <v>7</v>
+      </c>
+      <c r="B834" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A835" t="s">
+        <v>683</v>
+      </c>
+      <c r="B835" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A836" t="s">
+        <v>7</v>
+      </c>
+      <c r="B836" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A837" t="s">
+        <v>684</v>
+      </c>
+      <c r="B837" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A838" t="s">
+        <v>7</v>
+      </c>
+      <c r="B838" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A839" t="s">
+        <v>685</v>
+      </c>
+      <c r="B839" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A840" t="s">
+        <v>7</v>
+      </c>
+      <c r="B840" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A841" t="s">
+        <v>686</v>
+      </c>
+      <c r="B841" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A842" t="s">
+        <v>7</v>
+      </c>
+      <c r="B842" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A843" t="s">
+        <v>687</v>
+      </c>
+      <c r="B843" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A844" t="s">
+        <v>7</v>
+      </c>
+      <c r="B844" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A845" t="s">
         <v>616</v>
       </c>
     </row>
@@ -7888,9 +9256,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:B144"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="35.9375" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>